<commit_message>
it works with small batches and bigger delay
</commit_message>
<xml_diff>
--- a/EMAIL_SPAM_BOT/src/Emails/spam_emails.xlsx
+++ b/EMAIL_SPAM_BOT/src/Emails/spam_emails.xlsx
@@ -22,10 +22,10 @@
     <t>Email</t>
   </si>
   <si>
-    <t>5e140d92-6bf8-4ca9-ad3c-fde739ee94de</t>
+    <t>4705747a-8401-4484-9792-d9f6e63dabc2</t>
   </si>
   <si>
-    <t>ondra.losi@gmail.com</t>
+    <t>email.ads.ondrej@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>